<commit_message>
Add unit to GDP cell
</commit_message>
<xml_diff>
--- a/00_Input_files_for_damage_analysis/LUISA_damage_info_curves_template.xlsx
+++ b/00_Input_files_for_damage_analysis/LUISA_damage_info_curves_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/natalia_aleksandrova_deltares_nl/Documents/Documents/git_checkouts/CLIMAAX/FLOODS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecm5975/CLIMAAX/FLOODS/00_Input_files_for_damage_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="11_7BE859CF2764FA39C2903889AFA03F75A90CA07F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72D8F79D-6AD9-4547-BA72-2AB0C74620EF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91CE445-543D-7F40-B3D1-1A149068BDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="-26960" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>GDP/capita</t>
-  </si>
-  <si>
     <t>construction €/m²</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t>landuse content importance factor</t>
+  </si>
+  <si>
+    <t>GDP/capita US$</t>
   </si>
 </sst>
 </file>
@@ -524,10 +524,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -822,43 +818,43 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.85546875" style="17" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.28515625" style="17" customWidth="1"/>
-    <col min="10" max="11" width="8.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.83203125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.33203125" style="17" customWidth="1"/>
+    <col min="10" max="11" width="8.33203125" style="9" customWidth="1"/>
     <col min="12" max="12" width="18" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="18.28515625" style="8" customWidth="1"/>
-    <col min="20" max="20" width="26.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="18.33203125" style="8" customWidth="1"/>
+    <col min="20" max="20" width="26.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.5" style="6" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.33203125" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,111 +862,111 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="15" t="s">
+      <c r="M1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="R1" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="Y1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="22" t="s">
+      <c r="AA1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC1" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="AI1" s="5" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="26">
         <v>32169</v>
@@ -1081,12 +1077,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1121</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
         <f>C$2</f>
@@ -1198,12 +1194,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1122</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:C47" si="8">C$2</f>
@@ -1315,12 +1311,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1123</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="8"/>
@@ -1349,7 +1345,7 @@
         <v>26.776400000000002</v>
       </c>
       <c r="K5" s="16">
-        <f t="shared" ref="K3:K47" si="9">AA5*G5+AB5*H5+AC5*I5</f>
+        <f t="shared" ref="K5:K47" si="9">AA5*G5+AB5*H5+AC5*I5</f>
         <v>0.36108000000000001</v>
       </c>
       <c r="L5" s="3">
@@ -1432,12 +1428,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1130</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="8"/>
@@ -1549,12 +1545,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1210</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="8"/>
@@ -1666,12 +1662,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1221</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="8"/>
@@ -1783,12 +1779,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1222</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="8"/>
@@ -1900,12 +1896,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1230</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="8"/>
@@ -2017,12 +2013,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1241</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="8"/>
@@ -2134,12 +2130,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1242</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="8"/>
@@ -2251,12 +2247,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1310</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="8"/>
@@ -2368,12 +2364,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1320</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="8"/>
@@ -2485,12 +2481,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1330</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="8"/>
@@ -2602,12 +2598,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1410</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="8"/>
@@ -2719,12 +2715,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1421</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="8"/>
@@ -2836,12 +2832,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1422</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="8"/>
@@ -2953,12 +2949,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2110</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="8"/>
@@ -3071,12 +3067,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2120</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="8"/>
@@ -3189,12 +3185,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2130</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="8"/>
@@ -3307,12 +3303,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2210</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="8"/>
@@ -3425,12 +3421,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2220</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="8"/>
@@ -3543,12 +3539,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2230</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="8"/>
@@ -3661,12 +3657,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2310</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="8"/>
@@ -3779,12 +3775,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2410</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="8"/>
@@ -3897,12 +3893,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2420</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="8"/>
@@ -4015,12 +4011,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2430</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="8"/>
@@ -4133,12 +4129,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2440</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="8"/>
@@ -4251,12 +4247,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>3110</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="8"/>
@@ -4368,12 +4364,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>3120</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="8"/>
@@ -4485,12 +4481,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>3130</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="8"/>
@@ -4602,12 +4598,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>3210</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="8"/>
@@ -4719,12 +4715,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>3220</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="8"/>
@@ -4836,12 +4832,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>3230</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="8"/>
@@ -4953,12 +4949,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>3240</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="3">
         <f t="shared" si="8"/>
@@ -5070,12 +5066,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>3310</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" s="3">
         <f t="shared" si="8"/>
@@ -5187,12 +5183,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>3320</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" s="3">
         <f t="shared" si="8"/>
@@ -5304,12 +5300,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>3330</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" s="3">
         <f t="shared" si="8"/>
@@ -5421,12 +5417,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>3340</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="3">
         <f t="shared" si="8"/>
@@ -5538,12 +5534,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>3350</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" s="3">
         <f t="shared" si="8"/>
@@ -5655,12 +5651,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>4000</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="3">
         <f t="shared" si="8"/>
@@ -5772,12 +5768,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>5110</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" s="3">
         <f t="shared" si="8"/>
@@ -5889,12 +5885,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>5120</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="3">
         <f t="shared" si="8"/>
@@ -6006,12 +6002,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>5210</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" s="3">
         <f t="shared" si="8"/>
@@ -6123,12 +6119,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>5220</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" s="3">
         <f t="shared" si="8"/>
@@ -6240,12 +6236,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>5230</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="3">
         <f t="shared" si="8"/>

</xml_diff>